<commit_message>
Atualização automática de TAPEJARA.xlsx
</commit_message>
<xml_diff>
--- a/TAPEJARA.xlsx
+++ b/TAPEJARA.xlsx
@@ -8,25 +8,26 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gera-fichas\Comarcas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{480B0163-2F27-4E9D-814B-92EE63841616}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{CC2EDC51-6DF3-4AD0-B464-2E9CEC68E9C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Paineis DARQ" sheetId="7" r:id="rId1"/>
+    <sheet name="Paineis DARQ" sheetId="8" r:id="rId1"/>
     <sheet name="DESFAZIMENTOS" sheetId="1" r:id="rId2"/>
     <sheet name="MATERIAIS-FORNECIDOS" sheetId="2" r:id="rId3"/>
     <sheet name="DATA-LIMITE-REQUISICOES" sheetId="3" r:id="rId4"/>
     <sheet name="CPIP" sheetId="4" r:id="rId5"/>
     <sheet name="Recolhimento x Eliminacao" sheetId="5" r:id="rId6"/>
     <sheet name="Desarquivamentos Pendentes" sheetId="6" r:id="rId7"/>
+    <sheet name="DGC" sheetId="7" r:id="rId8"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="729" uniqueCount="300">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="735" uniqueCount="304">
   <si>
     <t>COMARCA</t>
   </si>
@@ -926,6 +927,18 @@
   </si>
   <si>
     <t>TAPEJARA</t>
+  </si>
+  <si>
+    <t>TEMÁTICA</t>
+  </si>
+  <si>
+    <t>PROBLEMA</t>
+  </si>
+  <si>
+    <t>MOT-Limpeza</t>
+  </si>
+  <si>
+    <t>Demora nos Atestes MOT</t>
   </si>
 </sst>
 </file>
@@ -935,7 +948,7 @@
   <numFmts count="1">
     <numFmt numFmtId="165" formatCode="&quot; &quot;mmmm&quot; / &quot;yyyy"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -988,6 +1001,19 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+    </font>
+    <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -1002,7 +1028,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1043,6 +1069,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFB7E1CD"/>
         <bgColor rgb="FFB7E1CD"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9D9D9"/>
+        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
     <fill>
@@ -1115,9 +1147,9 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1199,12 +1231,16 @@
     <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 3" xfId="1" xr:uid="{E1FD1BC8-D8E7-4A5E-A3C0-44A649AEC3D1}"/>
+    <cellStyle name="Normal 3" xfId="1" xr:uid="{026C8570-AF2C-4250-8E7F-058D8B4ED529}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1234,10 +1270,10 @@
         <xdr:cNvPr id="2" name="Chart1" title="Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{91D15FBC-4553-4782-AE3A-51EE3905C6DD}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1E10B471-1AA9-4D96-BC63-422E69D44625}"/>
             </a:ext>
             <a:ext uri="GoogleSheetsCustomDataVersion1">
-              <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="" pictureOfChart="1"/>
+              <go:sheetsCustomData xmlns="" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:go="http://customooxmlschemas.google.com/" pictureOfChart="1"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1275,7 +1311,7 @@
         <xdr:cNvPr id="3" name="Shape 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{607E5533-5D23-452B-93C5-DEF2AC643D35}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{517BE06A-4C9C-4AE2-9DDD-D2A0257CDA0C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1338,7 +1374,7 @@
         <xdr:cNvPr id="4" name="Shape 2" title="Desenho">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{24BA2959-B630-4549-BC34-7A38D520EF54}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EBE9EAEF-5D86-4D72-B8C5-BBD8889D3135}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1357,7 +1393,7 @@
           <xdr:cNvPr id="5" name="Shape 4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C9FD509B-1916-272C-0D5D-30C5E4E14D44}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4DDF8160-66D3-7EFB-A766-2C15FB3EB3C1}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1406,7 +1442,7 @@
           <xdr:cNvPr id="6" name="Shape 5">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{44CDB247-D414-F48B-7086-8BC035ED8AB3}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1C11DA89-0518-59F9-6CBA-FA3F1AD517F0}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1425,7 +1461,7 @@
             <xdr:cNvPr id="7" name="Shape 6">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E025AD9F-FAE2-15FB-EFEB-1D6ACED2D45F}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DD32B805-85A6-FD37-CC7D-052311F16AA1}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1456,7 +1492,7 @@
             <xdr:cNvPr id="8" name="Shape 7">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1F0AF098-4C77-10D7-FEBF-37CD92504EBC}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{583A70A5-DC2B-9E71-8D53-624C2A521ADE}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1487,7 +1523,7 @@
             <xdr:cNvPr id="9" name="Shape 8">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B3C93963-19E7-3E3C-45F1-C7D1DDCF4B03}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9B937AB4-6147-2932-307C-CC64B8F90E55}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1530,7 +1566,7 @@
         <xdr:cNvPr id="10" name="image2.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{46D8E843-4C7C-4544-98FB-E5E682337173}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E3598E90-FA40-45C3-9C2D-9C7D7AAF0AEC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1568,7 +1604,7 @@
         <xdr:cNvPr id="11" name="image1.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{44676360-7257-4337-9E56-96F3407D051D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9E17BB9F-0FE4-4633-A859-139F7211AF10}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1611,7 +1647,7 @@
         <xdr:cNvPr id="12" name="Imagem 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9256CD8B-23DC-4600-88ED-405600F809DE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0E439DFB-103C-4497-A0B5-AFB445356B99}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1924,7 +1960,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96D37809-3986-4FAD-959E-635485FC2137}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74A58B20-561F-44AF-8B54-226BAD6DA40D}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -1936,98 +1972,98 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="5" width="12.5703125" style="34"/>
-    <col min="6" max="6" width="2" style="34" customWidth="1"/>
-    <col min="7" max="16" width="13.42578125" style="34" customWidth="1"/>
-    <col min="17" max="16384" width="12.5703125" style="34"/>
+    <col min="1" max="5" width="12.5703125" style="36"/>
+    <col min="6" max="6" width="2" style="36" customWidth="1"/>
+    <col min="7" max="16" width="13.42578125" style="36" customWidth="1"/>
+    <col min="17" max="16384" width="12.5703125" style="36"/>
   </cols>
   <sheetData>
     <row r="1" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F1" s="33"/>
+      <c r="F1" s="35"/>
     </row>
     <row r="2" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F2" s="33"/>
+      <c r="F2" s="35"/>
     </row>
     <row r="3" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F3" s="33"/>
+      <c r="F3" s="35"/>
     </row>
     <row r="4" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F4" s="33"/>
+      <c r="F4" s="35"/>
     </row>
     <row r="5" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F5" s="33"/>
+      <c r="F5" s="35"/>
     </row>
     <row r="6" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F6" s="33"/>
+      <c r="F6" s="35"/>
     </row>
     <row r="7" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F7" s="33"/>
+      <c r="F7" s="35"/>
     </row>
     <row r="8" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F8" s="33"/>
+      <c r="F8" s="35"/>
     </row>
     <row r="9" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F9" s="33"/>
+      <c r="F9" s="35"/>
     </row>
     <row r="10" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F10" s="33"/>
+      <c r="F10" s="35"/>
     </row>
     <row r="11" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F11" s="33"/>
+      <c r="F11" s="35"/>
     </row>
     <row r="12" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F12" s="33"/>
+      <c r="F12" s="35"/>
     </row>
     <row r="13" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F13" s="33"/>
+      <c r="F13" s="35"/>
     </row>
     <row r="14" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F14" s="33"/>
+      <c r="F14" s="35"/>
     </row>
     <row r="15" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F15" s="33"/>
+      <c r="F15" s="35"/>
     </row>
     <row r="16" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F16" s="33"/>
+      <c r="F16" s="35"/>
     </row>
     <row r="17" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F17" s="33"/>
+      <c r="F17" s="35"/>
     </row>
     <row r="18" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F18" s="33"/>
+      <c r="F18" s="35"/>
     </row>
     <row r="19" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F19" s="33"/>
+      <c r="F19" s="35"/>
     </row>
     <row r="20" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F20" s="33"/>
+      <c r="F20" s="35"/>
     </row>
     <row r="21" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F21" s="33"/>
+      <c r="F21" s="35"/>
     </row>
     <row r="22" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F22" s="33"/>
+      <c r="F22" s="35"/>
     </row>
     <row r="23" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F23" s="33"/>
+      <c r="F23" s="35"/>
     </row>
     <row r="24" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F24" s="33"/>
+      <c r="F24" s="35"/>
     </row>
     <row r="25" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F25" s="33"/>
+      <c r="F25" s="35"/>
     </row>
     <row r="26" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F26" s="33"/>
+      <c r="F26" s="35"/>
     </row>
     <row r="27" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F27" s="33"/>
+      <c r="F27" s="35"/>
     </row>
     <row r="28" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F28" s="33"/>
+      <c r="F28" s="35"/>
     </row>
     <row r="29" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F29" s="33"/>
+      <c r="F29" s="35"/>
     </row>
   </sheetData>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -5508,4 +5544,44 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26.42578125" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" customWidth="1"/>
+    <col min="3" max="3" width="88.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="33" t="s">
+        <v>300</v>
+      </c>
+      <c r="C1" s="33" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="34" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="34" t="s">
+        <v>302</v>
+      </c>
+      <c r="C2" s="34" t="s">
+        <v>303</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>